<commit_message>
新增 interal index 的實驗
</commit_message>
<xml_diff>
--- a/log/clustering_log/clustering sumary.xlsx
+++ b/log/clustering_log/clustering sumary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZhongTing\Desktop\HotTopicDetection\log\clustering_log\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\宗廷\Desktop\HotTopicDetection\log\clustering_log\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="compare sampling=True times=25" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -48,9 +48,6 @@
     <t>ARI</t>
   </si>
   <si>
-    <t>test finished in 2685.33 seconds</t>
-  </si>
-  <si>
     <t>誤差線</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -63,26 +60,25 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>method1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
+    <t>clustering1</t>
   </si>
   <si>
-    <t>method2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
+    <t>clustering2</t>
   </si>
   <si>
-    <t>method3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
+    <t>clustering3</t>
   </si>
   <si>
-    <t>method4</t>
-    <phoneticPr fontId="18" type="noConversion"/>
+    <t>clustering4</t>
+  </si>
+  <si>
+    <t>test finished in 2918.06 seconds</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -732,7 +728,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="zh-TW"/>
   <c:roundedCorners val="0"/>
@@ -817,7 +813,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>method1</c:v>
+                  <c:v>clustering1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -843,19 +839,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>3.0000000000000027E-2</c:v>
+                    <c:v>2.9999999999999916E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.0000000000000027E-2</c:v>
+                    <c:v>2.9999999999999916E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.0000000000000018E-2</c:v>
+                    <c:v>2.9999999999999916E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>2.9999999999999916E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>3.9999999999999925E-2</c:v>
+                    <c:v>6.9999999999999951E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -867,19 +863,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>2.9999999999999916E-2</c:v>
+                    <c:v>5.0000000000000044E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.9999999999999916E-2</c:v>
+                    <c:v>8.0000000000000071E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.9999999999999907E-2</c:v>
+                    <c:v>7.0000000000000062E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.0000000000000018E-2</c:v>
+                    <c:v>9.000000000000008E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>9.000000000000008E-2</c:v>
+                    <c:v>0.20000000000000007</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -928,24 +924,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.94</c:v>
+                  <c:v>0.93</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.94</c:v>
+                  <c:v>0.93</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.94</c:v>
+                  <c:v>0.93</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.93</c:v>
+                  <c:v>0.92</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.92</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5C00-4F22-906A-E6E44204D3CA}"/>
             </c:ext>
@@ -960,7 +956,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>method2</c:v>
+                  <c:v>clustering2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -986,7 +982,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>2.9999999999999916E-2</c:v>
+                    <c:v>3.9999999999999925E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>3.0000000000000027E-2</c:v>
@@ -995,10 +991,10 @@
                     <c:v>2.9999999999999916E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.9999999999999907E-2</c:v>
+                    <c:v>3.9999999999999925E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.9999999999999916E-2</c:v>
+                    <c:v>6.9999999999999951E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1010,19 +1006,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>4.0000000000000036E-2</c:v>
+                    <c:v>6.0000000000000053E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.9999999999999907E-2</c:v>
+                    <c:v>4.9999999999999933E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.0000000000000018E-2</c:v>
+                    <c:v>5.0000000000000044E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>6.0000000000000053E-2</c:v>
+                    <c:v>7.0000000000000062E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>8.0000000000000071E-2</c:v>
+                    <c:v>0.12</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1071,7 +1067,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.92</c:v>
+                  <c:v>0.91</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.94</c:v>
@@ -1080,15 +1076,15 @@
                   <c:v>0.93</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.92</c:v>
+                  <c:v>0.91</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.92</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-5C00-4F22-906A-E6E44204D3CA}"/>
             </c:ext>
@@ -1103,7 +1099,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>method3</c:v>
+                  <c:v>clustering3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1138,10 +1134,10 @@
                     <c:v>2.9999999999999916E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.9999999999999907E-2</c:v>
+                    <c:v>3.9999999999999925E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.9999999999999916E-2</c:v>
+                    <c:v>6.9999999999999951E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1156,16 +1152,16 @@
                     <c:v>4.0000000000000036E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.9999999999999916E-2</c:v>
+                    <c:v>4.9999999999999933E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.0000000000000018E-2</c:v>
+                    <c:v>5.0000000000000044E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>4.0000000000000036E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>8.0000000000000071E-2</c:v>
+                    <c:v>0.12</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1214,7 +1210,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.93</c:v>
+                  <c:v>0.92</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.94</c:v>
@@ -1223,15 +1219,15 @@
                   <c:v>0.93</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.92</c:v>
+                  <c:v>0.91</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.92</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-5C00-4F22-906A-E6E44204D3CA}"/>
             </c:ext>
@@ -1246,7 +1242,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>method4</c:v>
+                  <c:v>clustering4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1275,16 +1271,16 @@
                     <c:v>3.9999999999999925E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.9999999999999916E-2</c:v>
+                    <c:v>2.0000000000000018E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>2.9999999999999916E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.0000000000000027E-2</c:v>
+                    <c:v>3.9999999999999925E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.9999999999999942E-2</c:v>
+                    <c:v>4.9999999999999933E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1299,10 +1295,10 @@
                     <c:v>5.0000000000000044E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>4.0000000000000036E-2</c:v>
+                    <c:v>3.9999999999999925E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.0000000000000036E-2</c:v>
+                    <c:v>3.0000000000000027E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>5.0000000000000044E-2</c:v>
@@ -1357,24 +1353,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.91</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>0.91</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.91</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-5C00-4F22-906A-E6E44204D3CA}"/>
             </c:ext>
@@ -1390,9 +1386,9 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="172526832"/>
-        <c:axId val="172531184"/>
-        <c:extLst>
+        <c:axId val="305664816"/>
+        <c:axId val="305661552"/>
+        <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
               <c15:ser>
@@ -1400,7 +1396,7 @@
                 <c:order val="0"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'compare sampling=True times=25'!$A$2</c15:sqref>
@@ -1445,7 +1441,7 @@
                 </c:errBars>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'compare sampling=True times=25'!$B$1:$F$1</c15:sqref>
@@ -1474,7 +1470,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'compare sampling=True times=25'!$B$2:$F$2</c15:sqref>
@@ -1487,7 +1483,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000A-5C00-4F22-906A-E6E44204D3CA}"/>
                   </c:ext>
@@ -1498,7 +1494,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="172526832"/>
+        <c:axId val="305664816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1541,7 +1537,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="172531184"/>
+        <c:crossAx val="305661552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1549,7 +1545,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="172531184"/>
+        <c:axId val="305661552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1658,7 +1654,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="172526832"/>
+        <c:crossAx val="305664816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2584,8 +2580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2614,30 +2610,30 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
-        <v>0.94</v>
+        <v>0.93</v>
       </c>
       <c r="C3">
-        <v>0.94</v>
+        <v>0.93</v>
       </c>
       <c r="D3">
-        <v>0.94</v>
+        <v>0.93</v>
       </c>
       <c r="E3">
-        <v>0.93</v>
+        <v>0.92</v>
       </c>
       <c r="F3">
-        <v>0.92</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4">
-        <v>0.92</v>
+        <v>0.91</v>
       </c>
       <c r="C4">
         <v>0.94</v>
@@ -2646,18 +2642,18 @@
         <v>0.93</v>
       </c>
       <c r="E4">
-        <v>0.92</v>
+        <v>0.91</v>
       </c>
       <c r="F4">
-        <v>0.92</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5">
-        <v>0.93</v>
+        <v>0.92</v>
       </c>
       <c r="C5">
         <v>0.94</v>
@@ -2666,30 +2662,30 @@
         <v>0.93</v>
       </c>
       <c r="E5">
-        <v>0.92</v>
+        <v>0.91</v>
       </c>
       <c r="F5">
-        <v>0.92</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6">
+        <v>0.92</v>
+      </c>
+      <c r="C6">
+        <v>0.94</v>
+      </c>
+      <c r="D6">
+        <v>0.93</v>
+      </c>
+      <c r="E6">
         <v>0.91</v>
       </c>
-      <c r="C6">
+      <c r="F6">
         <v>0.91</v>
-      </c>
-      <c r="D6">
-        <v>0.91</v>
-      </c>
-      <c r="E6">
-        <v>0.9</v>
-      </c>
-      <c r="F6">
-        <v>0.88</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2699,27 +2695,27 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8">
-        <v>0.97</v>
+        <v>0.96</v>
       </c>
       <c r="C8">
-        <v>0.97</v>
+        <v>0.96</v>
       </c>
       <c r="D8">
         <v>0.96</v>
       </c>
       <c r="E8">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
       <c r="F8">
-        <v>0.96</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>0.95</v>
@@ -2731,18 +2727,18 @@
         <v>0.96</v>
       </c>
       <c r="E9">
-        <v>0.94</v>
+        <v>0.95</v>
       </c>
       <c r="F9">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
       <c r="C10">
         <v>0.97</v>
@@ -2751,30 +2747,30 @@
         <v>0.96</v>
       </c>
       <c r="E10">
-        <v>0.94</v>
+        <v>0.95</v>
       </c>
       <c r="F10">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11">
+        <v>0.96</v>
+      </c>
+      <c r="C11">
+        <v>0.96</v>
+      </c>
+      <c r="D11">
+        <v>0.96</v>
+      </c>
+      <c r="E11">
         <v>0.95</v>
       </c>
-      <c r="C11">
-        <v>0.94</v>
-      </c>
-      <c r="D11">
-        <v>0.94</v>
-      </c>
-      <c r="E11">
-        <v>0.93</v>
-      </c>
       <c r="F11">
-        <v>0.94</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2784,85 +2780,85 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>0.91</v>
+        <v>0.88</v>
       </c>
       <c r="C13">
-        <v>0.91</v>
+        <v>0.85</v>
       </c>
       <c r="D13">
-        <v>0.92</v>
+        <v>0.86</v>
       </c>
       <c r="E13">
-        <v>0.91</v>
+        <v>0.83</v>
       </c>
       <c r="F13">
-        <v>0.83</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
+        <v>0.85</v>
+      </c>
+      <c r="C14">
+        <v>0.89</v>
+      </c>
+      <c r="D14">
         <v>0.88</v>
       </c>
-      <c r="C14">
-        <v>0.92</v>
-      </c>
-      <c r="D14">
-        <v>0.91</v>
-      </c>
       <c r="E14">
-        <v>0.86</v>
+        <v>0.84</v>
       </c>
       <c r="F14">
-        <v>0.84</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
+        <v>0.88</v>
+      </c>
+      <c r="C15">
         <v>0.89</v>
       </c>
-      <c r="C15">
-        <v>0.91</v>
-      </c>
       <c r="D15">
-        <v>0.91</v>
+        <v>0.88</v>
       </c>
       <c r="E15">
-        <v>0.88</v>
+        <v>0.87</v>
       </c>
       <c r="F15">
-        <v>0.84</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
+        <v>0.87</v>
+      </c>
+      <c r="C16">
+        <v>0.9</v>
+      </c>
+      <c r="D16">
+        <v>0.9</v>
+      </c>
+      <c r="E16">
         <v>0.86</v>
       </c>
-      <c r="C16">
-        <v>0.87</v>
-      </c>
-      <c r="D16">
-        <v>0.87</v>
-      </c>
-      <c r="E16">
-        <v>0.85</v>
-      </c>
       <c r="F16">
-        <v>0.77</v>
+        <v>0.8</v>
       </c>
       <c r="I16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -2870,19 +2866,19 @@
         <v>3</v>
       </c>
       <c r="I17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J17">
         <f>B8-B3</f>
-        <v>3.0000000000000027E-2</v>
+        <v>2.9999999999999916E-2</v>
       </c>
       <c r="K17">
         <f t="shared" ref="K17:N17" si="0">C8-C3</f>
-        <v>3.0000000000000027E-2</v>
+        <v>2.9999999999999916E-2</v>
       </c>
       <c r="L17">
         <f t="shared" si="0"/>
-        <v>2.0000000000000018E-2</v>
+        <v>2.9999999999999916E-2</v>
       </c>
       <c r="M17">
         <f t="shared" si="0"/>
@@ -2890,132 +2886,132 @@
       </c>
       <c r="N17">
         <f t="shared" si="0"/>
-        <v>3.9999999999999925E-2</v>
+        <v>6.9999999999999951E-2</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B18">
         <v>0.02</v>
       </c>
       <c r="C18">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="D18">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="E18">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="F18">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="J18">
-        <f t="shared" ref="J18:J21" si="1">B9-B4</f>
+        <f>B9-B4</f>
+        <v>3.9999999999999925E-2</v>
+      </c>
+      <c r="K18">
+        <f t="shared" ref="K18:N18" si="1">C9-C4</f>
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="1"/>
         <v>2.9999999999999916E-2</v>
       </c>
-      <c r="K18">
-        <f t="shared" ref="K18:K21" si="2">C9-C4</f>
-        <v>3.0000000000000027E-2</v>
-      </c>
-      <c r="L18">
-        <f t="shared" ref="L18:L21" si="3">D9-D4</f>
-        <v>2.9999999999999916E-2</v>
-      </c>
       <c r="M18">
-        <f t="shared" ref="M18:M21" si="4">E9-E4</f>
-        <v>1.9999999999999907E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.9999999999999925E-2</v>
       </c>
       <c r="N18">
-        <f t="shared" ref="N18:N21" si="5">F9-F4</f>
-        <v>2.9999999999999916E-2</v>
+        <f t="shared" si="1"/>
+        <v>6.9999999999999951E-2</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19">
         <v>0.02</v>
       </c>
       <c r="C19">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="D19">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="E19">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="F19">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="J19">
-        <f t="shared" si="1"/>
+        <f>B10-B5</f>
         <v>2.9999999999999916E-2</v>
       </c>
       <c r="K19">
+        <f t="shared" ref="K19:N19" si="2">C10-C5</f>
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="L19">
         <f t="shared" si="2"/>
-        <v>3.0000000000000027E-2</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="3"/>
         <v>2.9999999999999916E-2</v>
       </c>
       <c r="M19">
-        <f t="shared" si="4"/>
-        <v>1.9999999999999907E-2</v>
+        <f t="shared" si="2"/>
+        <v>3.9999999999999925E-2</v>
       </c>
       <c r="N19">
-        <f t="shared" si="5"/>
-        <v>2.9999999999999916E-2</v>
+        <f t="shared" si="2"/>
+        <v>6.9999999999999951E-2</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20">
         <v>0.02</v>
       </c>
       <c r="C20">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="D20">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="E20">
         <v>0.02</v>
       </c>
       <c r="F20">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="J20">
-        <f t="shared" si="1"/>
+        <f>B11-B6</f>
         <v>3.9999999999999925E-2</v>
       </c>
       <c r="K20">
-        <f t="shared" si="2"/>
-        <v>2.9999999999999916E-2</v>
+        <f t="shared" ref="K20:N20" si="3">C11-C6</f>
+        <v>2.0000000000000018E-2</v>
       </c>
       <c r="L20">
         <f t="shared" si="3"/>
         <v>2.9999999999999916E-2</v>
       </c>
       <c r="M20">
-        <f t="shared" si="4"/>
-        <v>3.0000000000000027E-2</v>
+        <f t="shared" si="3"/>
+        <v>3.9999999999999925E-2</v>
       </c>
       <c r="N20">
-        <f t="shared" si="5"/>
-        <v>5.9999999999999942E-2</v>
+        <f t="shared" si="3"/>
+        <v>4.9999999999999933E-2</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21">
         <v>0.02</v>
@@ -3035,66 +3031,66 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="I22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J22">
         <f>B3-B13</f>
-        <v>2.9999999999999916E-2</v>
+        <v>5.0000000000000044E-2</v>
       </c>
       <c r="K22">
-        <f t="shared" ref="K22:N27" si="6">C3-C13</f>
-        <v>2.9999999999999916E-2</v>
+        <f t="shared" ref="K22:N22" si="4">C3-C13</f>
+        <v>8.0000000000000071E-2</v>
       </c>
       <c r="L22">
-        <f t="shared" si="6"/>
-        <v>1.9999999999999907E-2</v>
+        <f>D3-D13</f>
+        <v>7.0000000000000062E-2</v>
       </c>
       <c r="M22">
-        <f t="shared" si="6"/>
-        <v>2.0000000000000018E-2</v>
+        <f t="shared" si="4"/>
+        <v>9.000000000000008E-2</v>
       </c>
       <c r="N22">
-        <f t="shared" si="6"/>
-        <v>9.000000000000008E-2</v>
+        <f t="shared" si="4"/>
+        <v>0.20000000000000007</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J23">
-        <f t="shared" ref="J23:J27" si="7">B4-B14</f>
-        <v>4.0000000000000036E-2</v>
+        <f>B4-B14</f>
+        <v>6.0000000000000053E-2</v>
       </c>
       <c r="K23">
-        <f t="shared" si="6"/>
-        <v>1.9999999999999907E-2</v>
+        <f t="shared" ref="K23:N23" si="5">C4-C14</f>
+        <v>4.9999999999999933E-2</v>
       </c>
       <c r="L23">
-        <f t="shared" si="6"/>
-        <v>2.0000000000000018E-2</v>
+        <f t="shared" si="5"/>
+        <v>5.0000000000000044E-2</v>
       </c>
       <c r="M23">
-        <f t="shared" si="6"/>
-        <v>6.0000000000000053E-2</v>
+        <f t="shared" si="5"/>
+        <v>7.0000000000000062E-2</v>
       </c>
       <c r="N23">
-        <f t="shared" si="6"/>
-        <v>8.0000000000000071E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.12</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J24">
-        <f t="shared" si="7"/>
+        <f>B5-B15</f>
         <v>4.0000000000000036E-2</v>
       </c>
       <c r="K24">
-        <f t="shared" si="6"/>
-        <v>2.9999999999999916E-2</v>
+        <f t="shared" ref="K24:N24" si="6">C5-C15</f>
+        <v>4.9999999999999933E-2</v>
       </c>
       <c r="L24">
         <f t="shared" si="6"/>
-        <v>2.0000000000000018E-2</v>
+        <v>5.0000000000000044E-2</v>
       </c>
       <c r="M24">
         <f t="shared" si="6"/>
@@ -3102,28 +3098,28 @@
       </c>
       <c r="N24">
         <f t="shared" si="6"/>
-        <v>8.0000000000000071E-2</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J25">
+        <f>B6-B16</f>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="K25">
+        <f t="shared" ref="K25:N25" si="7">C6-C16</f>
+        <v>3.9999999999999925E-2</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="7"/>
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="M25">
         <f t="shared" si="7"/>
         <v>5.0000000000000044E-2</v>
       </c>
-      <c r="K25">
-        <f t="shared" si="6"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="L25">
-        <f t="shared" si="6"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="M25">
-        <f t="shared" si="6"/>
-        <v>5.0000000000000044E-2</v>
-      </c>
       <c r="N25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.10999999999999999</v>
       </c>
     </row>

</xml_diff>